<commit_message>
add results for chaos and preprints
</commit_message>
<xml_diff>
--- a/results/results-main.xlsx
+++ b/results/results-main.xlsx
@@ -899,7 +899,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MASE</t>
+          <t>sMAPE</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -912,7 +912,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>sMAPE</t>
+          <t>MASE</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -925,7 +925,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>EV</t>
+          <t>percent error</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -938,7 +938,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>percent error</t>
+          <t>pearson correlation</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -951,7 +951,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>pearson correlation</t>
+          <t>EV</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -977,7 +977,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>AE</t>
+          <t>probabilistic interval performance metric used in the COVID-19 Forecast Hub</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -990,7 +990,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>probabilistic interval performance metric used in the COVID-19 Forecast Hub</t>
+          <t>MSPE</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -1003,7 +1003,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>CCC</t>
+          <t>RMdSPE</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -1016,7 +1016,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>BIC</t>
+          <t>ACD</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -1029,7 +1029,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>relative error</t>
+          <t>BIC</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -1042,7 +1042,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>DIC</t>
+          <t>CRPS</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -1055,7 +1055,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>AFER</t>
+          <t>ARE</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -1068,7 +1068,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>precision</t>
+          <t>interval scoring method (CI's that are too wide)</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -1081,7 +1081,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>ACD</t>
+          <t>CCC</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -1107,7 +1107,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>MSLE</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -1120,7 +1120,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>interval scoring method (CI's that are too wide)</t>
+          <t>precision</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -1133,7 +1133,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>nRMSE</t>
+          <t>AFER</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -1146,7 +1146,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>RMSPE</t>
+          <t>RMSD</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -1159,7 +1159,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>RMSLE</t>
+          <t>relative error</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -1172,7 +1172,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>MSLE</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -1198,7 +1198,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>RMSD</t>
+          <t>DIC</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -1211,7 +1211,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>ARE</t>
+          <t>MSIS</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -1224,7 +1224,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>MSPE</t>
+          <t>AE</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -1237,7 +1237,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>MSIS</t>
+          <t>RMSPE</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -1250,7 +1250,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>CRPS</t>
+          <t>nRMSE</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1276,7 +1276,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>RMdSPE</t>
+          <t>RMSLE</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1580,7 +1580,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>looks like there's some kind of PI</t>
+          <t>70% CIs</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -1593,7 +1593,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>75% CIs</t>
+          <t>exceedance probabilities (prob that true value will exceed a given value)</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -1606,7 +1606,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>80% PIs</t>
+          <t>95% PIs</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -1619,7 +1619,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>70% CIs</t>
+          <t>99% Upper and Lower Limit</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -1632,7 +1632,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>multiple CIs</t>
+          <t>some kind of PI. show full range of simulations that fall within a 10% error tolerance</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -1658,7 +1658,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>50% CIs</t>
+          <t>some kind of PIs</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -1671,7 +1671,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>exceedance probabilities (prob that true value will exceed a given value)</t>
+          <t>80% PIs</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -1697,7 +1697,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>some kind of PI. show full range of simulations that fall within a 10% error tolerance</t>
+          <t>some kind of PIs shown on plots but not specified what it is</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -1710,7 +1710,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>some kind of PIs shown on plots but not specified what it is</t>
+          <t>looks like there's some kind of PI</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -1723,7 +1723,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>99% Upper and Lower Limit</t>
+          <t>multiple CIs</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -1736,7 +1736,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>CIs/Pis</t>
+          <t>75% CIs</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -1762,7 +1762,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>some kind of PIs</t>
+          <t>some kind of PI</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -1775,7 +1775,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>95% PIs</t>
+          <t>50% CIs</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -1788,7 +1788,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>some kind of PI</t>
+          <t>CIs/Pis</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -2055,7 +2055,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PLOS ONE</t>
+          <t>Scientific Reports</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -2068,7 +2068,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Scientific Reports</t>
+          <t>PLOS ONE</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -2090,7 +2090,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>arXiv</t>
+          <t>Infectious Disease Modelling</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -2103,7 +2103,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Infectious Disease Modelling</t>
+          <t>arXiv</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -2155,7 +2155,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Nature Communications</t>
+          <t>Health &amp; Place</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -2168,7 +2168,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Results in Physics</t>
+          <t>Science of The Total Environment</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -2181,7 +2181,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>PLOS Computational Biology</t>
+          <t>Results in Physics</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -2194,7 +2194,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Science of The Total Environment</t>
+          <t>Nature Human Behaviour</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -2207,7 +2207,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Health &amp; Place</t>
+          <t>Computational Mechanics</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -2220,7 +2220,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Nature Human Behaviour</t>
+          <t>Nature Communications</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -2233,7 +2233,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Computational Mechanics</t>
+          <t>PLOS Computational Biology</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -2246,7 +2246,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Computers in Biology and Medicine</t>
+          <t>European Journal of Operational Research</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -2259,7 +2259,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Quality &amp; Quantity</t>
+          <t>JAMA Network Open</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -2272,7 +2272,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Nature Medicine</t>
+          <t>Proceedings of the Royal Society A: Mathematical, Physical and Engineering Sciences</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -2285,7 +2285,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Vaccine</t>
+          <t>Annual Reviews in Control</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -2298,7 +2298,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>International Orthopaedics</t>
+          <t>IEEE Transactions on Instrumentation and Measurement</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -2311,7 +2311,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Annual Reviews in Control</t>
+          <t>Soft Computing</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -2324,7 +2324,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Epidemics</t>
+          <t>Physica A: Statistical Mechanics and its Applications</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -2337,7 +2337,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Journal of Big Data</t>
+          <t>Chemical Engineering Journal</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -2350,7 +2350,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Journal of Travel Medicine</t>
+          <t>Physical Review X</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -2363,7 +2363,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Decision Support Systems</t>
+          <t>Journal of Biomedical Informatics</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -2376,7 +2376,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Emerging Infectious Diseases</t>
+          <t>Journal of Travel Medicine</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -2389,7 +2389,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>GigaScience</t>
+          <t>International Journal of Geographical Information Science</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -2402,7 +2402,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>American Journal of Public Health</t>
+          <t>Computer Methods in Applied Mechanics and Engineering</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -2415,7 +2415,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Computer Methods in Applied Mechanics and Engineering</t>
+          <t>Quality &amp; Quantity</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -2428,7 +2428,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>IEEE Transactions on Computational Social Systems</t>
+          <t>Mathematical Methods in the Applied Sciences</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -2441,7 +2441,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Chemical Engineering Journal</t>
+          <t>Epidemics</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -2454,7 +2454,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>European Journal of Operational Research</t>
+          <t>Journal of Big Data</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -2467,7 +2467,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Physical Review X</t>
+          <t>Journal of Theoretical Biology</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -2480,7 +2480,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>International Journal of Geographical Information Science</t>
+          <t>IEEE Transactions on Computational Social Systems</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -2493,7 +2493,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Mathematical Methods in the Applied Sciences</t>
+          <t>Computers in Biology and Medicine</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -2506,7 +2506,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Soft Computing</t>
+          <t>Decision Support Systems</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -2519,7 +2519,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Journal of Theoretical Biology</t>
+          <t>American Journal of Public Health</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -2532,7 +2532,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Physica A: Statistical Mechanics and its Applications</t>
+          <t>European Journal of Epidemiology</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -2545,7 +2545,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>IEEE Transactions on Instrumentation and Measurement</t>
+          <t>Vaccine</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -2558,7 +2558,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Journal of Biomedical Informatics</t>
+          <t>International Orthopaedics</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -2571,7 +2571,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Proceedings of the Royal Society A: Mathematical, Physical and Engineering Sciences</t>
+          <t>IEEE Journal of Biomedical and Health Informatics</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -2584,7 +2584,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>IEEE Journal of Biomedical and Health Informatics</t>
+          <t>Journal of the American Statistical Association</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -2597,7 +2597,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Expert Systems with Applications</t>
+          <t>Emerging Infectious Diseases</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -2610,7 +2610,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>JAMA Network Open</t>
+          <t>PLOS Biology</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -2623,7 +2623,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>PLOS Biology</t>
+          <t>American Journal of Preventive Medicine</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -2636,7 +2636,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Journal of Medical Virology</t>
+          <t>Expert Systems with Applications</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -2649,7 +2649,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>American Journal of Preventive Medicine</t>
+          <t>Journal of Medical Virology</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -2662,7 +2662,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>European Journal of Epidemiology</t>
+          <t>GigaScience</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -2675,7 +2675,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Journal of the American Statistical Association</t>
+          <t>Nature Medicine</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -2828,7 +2828,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>climate</t>
+          <t>human behavior</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -2841,7 +2841,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>human behavior</t>
+          <t>climate</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -2906,7 +2906,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>vaccination</t>
+          <t>wastewater concentration of covid</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -2919,7 +2919,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>wastewater concentration of covid</t>
+          <t>vaccination</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -3046,7 +3046,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Infectious Diseases</t>
+          <t>Electrical and Electronic Engineering</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -3059,7 +3059,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Electrical and Electronic Engineering</t>
+          <t>Infectious Diseases</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -3137,7 +3137,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Aerospace Engineering</t>
+          <t>Public Health, Environmental and Occupational Health</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -3150,7 +3150,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Public Health, Environmental and Occupational Health</t>
+          <t>Aerospace Engineering</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -3163,7 +3163,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Modelling and Simulation</t>
+          <t>General Biochemistry, Genetics and Molecular Biology</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -3176,7 +3176,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>General Biochemistry, Genetics and Molecular Biology</t>
+          <t>Modelling and Simulation</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -3202,7 +3202,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>General Medicine</t>
+          <t>Epidemiology</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -3215,7 +3215,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Epidemiology</t>
+          <t>Statistics and Probability</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -3228,7 +3228,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Instrumentation</t>
+          <t>General Medicine</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -3241,7 +3241,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Statistics and Probability</t>
+          <t>Instrumentation</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -3254,7 +3254,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Environmental Chemistry</t>
+          <t>Information Systems and Management</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -3267,7 +3267,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Geography, Planning and Development</t>
+          <t>General Engineering</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -3280,7 +3280,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Computational Mechanics</t>
+          <t>General Immunology and Microbiology</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -3293,7 +3293,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>General Immunology and Microbiology</t>
+          <t>General Chemistry</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -3306,7 +3306,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>General Chemistry</t>
+          <t>Environmental Chemistry</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -3319,7 +3319,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Information Systems</t>
+          <t>Health Informatics</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -3332,7 +3332,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>General Engineering</t>
+          <t>Computational Mechanics</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -3345,7 +3345,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Information Systems and Management</t>
+          <t>Information Systems</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -3358,7 +3358,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Health Informatics</t>
+          <t>Geography, Planning and Development</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -3371,7 +3371,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Behavioral Neuroscience</t>
+          <t>Virology</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -3384,7 +3384,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Cellular and Molecular Neuroscience</t>
+          <t>Genetics</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -3397,7 +3397,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Health(social science)</t>
+          <t>Social Psychology</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -3410,7 +3410,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Molecular Biology</t>
+          <t>Health(social science)</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -3423,7 +3423,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Environmental Engineering</t>
+          <t>Cellular and Molecular Neuroscience</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -3436,7 +3436,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Experimental and Cognitive Psychology</t>
+          <t>Environmental Engineering</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -3449,7 +3449,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Virology</t>
+          <t>Waste Management and Disposal</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -3462,7 +3462,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Ecology</t>
+          <t>Experimental and Cognitive Psychology</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -3475,7 +3475,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Industrial and Manufacturing Engineering</t>
+          <t>Behavioral Neuroscience</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -3488,7 +3488,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Pollution</t>
+          <t>Molecular Biology</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -3501,7 +3501,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Software</t>
+          <t>Pollution</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -3514,7 +3514,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>General Agricultural and Biological Sciences</t>
+          <t>Industrial and Manufacturing Engineering</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -3527,7 +3527,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Social Psychology</t>
+          <t>Ecology, Evolution, Behavior and Systematics</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -3540,7 +3540,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Waste Management and Disposal</t>
+          <t>Computational Mathematics</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -3553,7 +3553,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Computational Mathematics</t>
+          <t>General Agricultural and Biological Sciences</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -3566,7 +3566,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Genetics</t>
+          <t>Ecology</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -3579,7 +3579,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Ecology, Evolution, Behavior and Systematics</t>
+          <t>Software</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -3592,7 +3592,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Geometry and Topology</t>
+          <t>Arts and Humanities (miscellaneous)</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -3605,7 +3605,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Mechanics of Materials</t>
+          <t>Social Sciences (miscellaneous)</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -3618,7 +3618,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Library and Information Sciences</t>
+          <t>Computer Networks and Communications</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -3631,7 +3631,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Theoretical Computer Science</t>
+          <t>Microbiology (medical)</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -3644,7 +3644,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Developmental and Educational Psychology</t>
+          <t>General Chemical Engineering</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -3657,7 +3657,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Arts and Humanities (miscellaneous)</t>
+          <t>General Social Sciences</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -3670,7 +3670,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>General Neuroscience</t>
+          <t>Cognitive Neuroscience</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -3683,7 +3683,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Orthopedics and Sports Medicine</t>
+          <t>Management Science and Operations Research</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -3696,7 +3696,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Parasitology</t>
+          <t>General Computer Science</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -3709,7 +3709,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Management Science and Operations Research</t>
+          <t>Library and Information Sciences</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -3722,7 +3722,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Management Information Systems</t>
+          <t>Parasitology</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -3735,7 +3735,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>General Chemical Engineering</t>
+          <t>Molecular Medicine</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -3748,7 +3748,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Artificial Intelligence</t>
+          <t>Management Information Systems</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -3761,7 +3761,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Human-Computer Interaction</t>
+          <t>Artificial Intelligence</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -3774,7 +3774,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Statistics, Probability and Uncertainty</t>
+          <t>Condensed Matter Physics</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -3787,7 +3787,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Computer Vision and Pattern Recognition</t>
+          <t>Geometry and Topology</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -3800,7 +3800,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Health Information Management</t>
+          <t>Developmental and Educational Psychology</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -3813,7 +3813,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Microbiology</t>
+          <t>General Neuroscience</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -3826,7 +3826,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Social Sciences (miscellaneous)</t>
+          <t>Statistics, Probability and Uncertainty</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -3839,7 +3839,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Cognitive Neuroscience</t>
+          <t>General Veterinary</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -3852,7 +3852,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>General Computer Science</t>
+          <t>Surgery</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -3865,7 +3865,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>General Social Sciences</t>
+          <t>Health Information Management</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -3891,7 +3891,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Biotechnology</t>
+          <t>Orthopedics and Sports Medicine</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -3904,7 +3904,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Computer Networks and Communications</t>
+          <t>Computer Vision and Pattern Recognition</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -3917,7 +3917,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Condensed Matter Physics</t>
+          <t>Biotechnology</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -3930,7 +3930,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Surgery</t>
+          <t>Theoretical Computer Science</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -3943,7 +3943,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>General Veterinary</t>
+          <t>Mechanics of Materials</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -3956,7 +3956,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Molecular Medicine</t>
+          <t>Human-Computer Interaction</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -3969,7 +3969,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Microbiology (medical)</t>
+          <t>Microbiology</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -4497,7 +4497,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>zipcode</t>
+          <t>regional (within state)</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -4510,7 +4510,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>town</t>
+          <t>zipcode</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -4523,7 +4523,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>regional (within state)</t>
+          <t>town</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -4624,7 +4624,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>peak cases</t>
+          <t>growth rate</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -4637,7 +4637,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>growth rate</t>
+          <t>peak cases</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -4663,7 +4663,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>peak deaths</t>
+          <t>total deaths</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -4676,7 +4676,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>total deaths</t>
+          <t>peak deaths</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -4689,7 +4689,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>curves of probabilities that cases/deaths/recoveries will exceed certain values</t>
+          <t>critical care beds</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -4702,7 +4702,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>symptomatic cases</t>
+          <t>curves of probabilities that cases/deaths/recoveries will exceed certain values</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -4715,7 +4715,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>critical care beds</t>
+          <t>ventilators</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -4728,7 +4728,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>tests</t>
+          <t>duration of outbreak</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -4741,7 +4741,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>"spectral slope" (indicator of cases)</t>
+          <t>tests</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -4754,7 +4754,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>costs</t>
+          <t>"spectral slope" (indicator of cases)</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -4767,7 +4767,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>attack rate</t>
+          <t>costs</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -4780,7 +4780,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>parameters</t>
+          <t>peak ICU admissions</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -4793,7 +4793,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>end dates of pandemic</t>
+          <t>exposed</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -4806,7 +4806,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>duration of outbreak</t>
+          <t>end dates of pandemic</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -4819,7 +4819,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>exposed</t>
+          <t>symptomatic cases</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -4832,7 +4832,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>peak cases date</t>
+          <t>attack rate</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -4845,7 +4845,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>peak ICU admissions</t>
+          <t>peak cases date</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -4858,7 +4858,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>ventilators</t>
+          <t>parameters</t>
         </is>
       </c>
       <c r="B24" t="n">

</xml_diff>